<commit_message>
Query data from IIHS for legalized states
</commit_message>
<xml_diff>
--- a/data/USA-FatalCrashes.xlsx
+++ b/data/USA-FatalCrashes.xlsx
@@ -22,7 +22,7 @@
     <t>Fatal Motor Vehicle Crashes</t>
   </si>
   <si>
-    <t>Years: 2013-2022</t>
+    <t>Years: 2008-2022</t>
   </si>
   <si>
     <r>
@@ -349,7 +349,7 @@
   <sheetPr filterMode="0" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
     </sheetView>
@@ -457,489 +457,709 @@
     </row>
     <row r="8" ht="14" customHeight="1">
       <c r="A8" s="6">
-        <v>2013</v>
+        <v>2008</v>
       </c>
       <c r="B8" s="7">
-        <v>2230</v>
+        <v>2575</v>
       </c>
       <c r="C8" s="7">
-        <v>1952</v>
+        <v>2586</v>
       </c>
       <c r="D8" s="7">
-        <v>2356</v>
+        <v>2549</v>
       </c>
       <c r="E8" s="7">
-        <v>2300</v>
+        <v>2722</v>
       </c>
       <c r="F8" s="7">
-        <v>2532</v>
+        <v>2887</v>
       </c>
       <c r="G8" s="7">
-        <v>2692</v>
+        <v>3029</v>
       </c>
       <c r="H8" s="7">
-        <v>2660</v>
+        <v>3018</v>
       </c>
       <c r="I8" s="7">
-        <v>2899</v>
+        <v>3224</v>
       </c>
       <c r="J8" s="7">
-        <v>2741</v>
+        <v>2860</v>
       </c>
       <c r="K8" s="7">
-        <v>2768</v>
+        <v>3063</v>
       </c>
       <c r="L8" s="7">
-        <v>2615</v>
+        <v>2829</v>
       </c>
       <c r="M8" s="7">
-        <v>2457</v>
+        <v>2830</v>
       </c>
       <c r="N8" s="7">
-        <v>30202</v>
+        <v>34172</v>
       </c>
     </row>
     <row r="9" ht="14" customHeight="1">
       <c r="A9" s="6">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="B9" s="7">
-        <v>2168</v>
+        <v>2377</v>
       </c>
       <c r="C9" s="7">
-        <v>1893</v>
+        <v>2167</v>
       </c>
       <c r="D9" s="7">
-        <v>2245</v>
+        <v>2349</v>
       </c>
       <c r="E9" s="7">
-        <v>2308</v>
+        <v>2592</v>
       </c>
       <c r="F9" s="7">
-        <v>2596</v>
+        <v>2780</v>
       </c>
       <c r="G9" s="7">
-        <v>2583</v>
+        <v>2750</v>
       </c>
       <c r="H9" s="7">
-        <v>2696</v>
+        <v>2787</v>
       </c>
       <c r="I9" s="7">
-        <v>2800</v>
+        <v>2865</v>
       </c>
       <c r="J9" s="7">
-        <v>2618</v>
+        <v>2650</v>
       </c>
       <c r="K9" s="7">
-        <v>2831</v>
+        <v>2622</v>
       </c>
       <c r="L9" s="7">
-        <v>2714</v>
+        <v>2512</v>
       </c>
       <c r="M9" s="7">
-        <v>2604</v>
+        <v>2411</v>
       </c>
       <c r="N9" s="7">
-        <v>30056</v>
+        <v>30862</v>
       </c>
     </row>
     <row r="10" ht="14" customHeight="1">
       <c r="A10" s="6">
-        <v>2015</v>
+        <v>2010</v>
       </c>
       <c r="B10" s="7">
-        <v>2371</v>
+        <v>2101</v>
       </c>
       <c r="C10" s="7">
-        <v>1983</v>
+        <v>1830</v>
       </c>
       <c r="D10" s="7">
-        <v>2401</v>
+        <v>2213</v>
       </c>
       <c r="E10" s="7">
-        <v>2439</v>
+        <v>2552</v>
       </c>
       <c r="F10" s="7">
-        <v>2869</v>
+        <v>2704</v>
       </c>
       <c r="G10" s="7">
-        <v>2790</v>
+        <v>2569</v>
       </c>
       <c r="H10" s="7">
-        <v>3021</v>
+        <v>2852</v>
       </c>
       <c r="I10" s="7">
-        <v>3049</v>
+        <v>2825</v>
       </c>
       <c r="J10" s="7">
-        <v>2904</v>
+        <v>2799</v>
       </c>
       <c r="K10" s="7">
-        <v>3070</v>
+        <v>2827</v>
       </c>
       <c r="L10" s="7">
-        <v>2780</v>
+        <v>2587</v>
       </c>
       <c r="M10" s="7">
-        <v>2861</v>
+        <v>2437</v>
       </c>
       <c r="N10" s="7">
-        <v>32538</v>
+        <v>30296</v>
       </c>
     </row>
     <row r="11" ht="14" customHeight="1">
       <c r="A11" s="6">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="B11" s="7">
-        <v>2354</v>
+        <v>2088</v>
       </c>
       <c r="C11" s="7">
-        <v>2426</v>
+        <v>1880</v>
       </c>
       <c r="D11" s="7">
-        <v>2694</v>
+        <v>2220</v>
       </c>
       <c r="E11" s="7">
-        <v>2713</v>
+        <v>2338</v>
       </c>
       <c r="F11" s="7">
-        <v>3005</v>
+        <v>2578</v>
       </c>
       <c r="G11" s="7">
-        <v>3025</v>
+        <v>2624</v>
       </c>
       <c r="H11" s="7">
-        <v>3025</v>
+        <v>2910</v>
       </c>
       <c r="I11" s="7">
-        <v>3134</v>
+        <v>2749</v>
       </c>
       <c r="J11" s="7">
-        <v>3154</v>
+        <v>2633</v>
       </c>
       <c r="K11" s="7">
-        <v>3287</v>
+        <v>2856</v>
       </c>
       <c r="L11" s="7">
-        <v>3041</v>
+        <v>2494</v>
       </c>
       <c r="M11" s="7">
-        <v>2890</v>
+        <v>2497</v>
       </c>
       <c r="N11" s="7">
-        <v>34748</v>
+        <v>29867</v>
       </c>
     </row>
     <row r="12" ht="14" customHeight="1">
       <c r="A12" s="6">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="B12" s="7">
-        <v>2625</v>
+        <v>2283</v>
       </c>
       <c r="C12" s="7">
-        <v>2312</v>
+        <v>2127</v>
       </c>
       <c r="D12" s="7">
-        <v>2689</v>
+        <v>2487</v>
       </c>
       <c r="E12" s="7">
-        <v>2770</v>
+        <v>2434</v>
       </c>
       <c r="F12" s="7">
-        <v>2915</v>
+        <v>2672</v>
       </c>
       <c r="G12" s="7">
-        <v>3032</v>
+        <v>2789</v>
       </c>
       <c r="H12" s="7">
-        <v>3237</v>
+        <v>2833</v>
       </c>
       <c r="I12" s="7">
-        <v>2990</v>
+        <v>2844</v>
       </c>
       <c r="J12" s="7">
-        <v>3108</v>
+        <v>2735</v>
       </c>
       <c r="K12" s="7">
-        <v>3107</v>
+        <v>2658</v>
       </c>
       <c r="L12" s="7">
-        <v>2903</v>
+        <v>2602</v>
       </c>
       <c r="M12" s="7">
-        <v>2872</v>
+        <v>2542</v>
       </c>
       <c r="N12" s="7">
-        <v>34560</v>
+        <v>31006</v>
       </c>
     </row>
     <row r="13" ht="14" customHeight="1">
       <c r="A13" s="6">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B13" s="7">
-        <v>2631</v>
+        <v>2230</v>
       </c>
       <c r="C13" s="7">
-        <v>2320</v>
+        <v>1952</v>
       </c>
       <c r="D13" s="7">
+        <v>2356</v>
+      </c>
+      <c r="E13" s="7">
+        <v>2300</v>
+      </c>
+      <c r="F13" s="7">
+        <v>2532</v>
+      </c>
+      <c r="G13" s="7">
+        <v>2692</v>
+      </c>
+      <c r="H13" s="7">
+        <v>2660</v>
+      </c>
+      <c r="I13" s="7">
+        <v>2899</v>
+      </c>
+      <c r="J13" s="7">
+        <v>2741</v>
+      </c>
+      <c r="K13" s="7">
+        <v>2768</v>
+      </c>
+      <c r="L13" s="7">
         <v>2615</v>
       </c>
-      <c r="E13" s="7">
-        <v>2572</v>
-      </c>
-      <c r="F13" s="7">
-        <v>2977</v>
-      </c>
-      <c r="G13" s="7">
-        <v>3026</v>
-      </c>
-      <c r="H13" s="7">
-        <v>3056</v>
-      </c>
-      <c r="I13" s="7">
-        <v>3009</v>
-      </c>
-      <c r="J13" s="7">
-        <v>3064</v>
-      </c>
-      <c r="K13" s="7">
-        <v>3108</v>
-      </c>
-      <c r="L13" s="7">
-        <v>2791</v>
-      </c>
       <c r="M13" s="7">
-        <v>2750</v>
+        <v>2457</v>
       </c>
       <c r="N13" s="7">
-        <v>33919</v>
+        <v>30202</v>
       </c>
     </row>
     <row r="14" ht="14" customHeight="1">
       <c r="A14" s="6">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="B14" s="7">
-        <v>2476</v>
+        <v>2168</v>
       </c>
       <c r="C14" s="7">
-        <v>2205</v>
+        <v>1893</v>
       </c>
       <c r="D14" s="7">
-        <v>2544</v>
+        <v>2245</v>
       </c>
       <c r="E14" s="7">
-        <v>2611</v>
+        <v>2308</v>
       </c>
       <c r="F14" s="7">
-        <v>2917</v>
+        <v>2596</v>
       </c>
       <c r="G14" s="7">
-        <v>2926</v>
+        <v>2583</v>
       </c>
       <c r="H14" s="7">
-        <v>3037</v>
+        <v>2696</v>
       </c>
       <c r="I14" s="7">
-        <v>3091</v>
+        <v>2800</v>
       </c>
       <c r="J14" s="7">
-        <v>3093</v>
+        <v>2618</v>
       </c>
       <c r="K14" s="7">
-        <v>2972</v>
+        <v>2831</v>
       </c>
       <c r="L14" s="7">
-        <v>2841</v>
+        <v>2714</v>
       </c>
       <c r="M14" s="7">
-        <v>2774</v>
+        <v>2604</v>
       </c>
       <c r="N14" s="7">
-        <v>33487</v>
+        <v>30056</v>
       </c>
     </row>
     <row r="15" ht="14" customHeight="1">
       <c r="A15" s="6">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="B15" s="7">
-        <v>2486</v>
+        <v>2371</v>
       </c>
       <c r="C15" s="7">
-        <v>2453</v>
+        <v>1983</v>
       </c>
       <c r="D15" s="7">
-        <v>2375</v>
+        <v>2401</v>
       </c>
       <c r="E15" s="7">
-        <v>2130</v>
+        <v>2439</v>
       </c>
       <c r="F15" s="7">
-        <v>2876</v>
+        <v>2869</v>
       </c>
       <c r="G15" s="7">
-        <v>3380</v>
+        <v>2790</v>
       </c>
       <c r="H15" s="7">
-        <v>3489</v>
+        <v>3021</v>
       </c>
       <c r="I15" s="7">
-        <v>3539</v>
+        <v>3049</v>
       </c>
       <c r="J15" s="7">
-        <v>3447</v>
+        <v>2904</v>
       </c>
       <c r="K15" s="7">
-        <v>3542</v>
+        <v>3070</v>
       </c>
       <c r="L15" s="7">
-        <v>3204</v>
+        <v>2780</v>
       </c>
       <c r="M15" s="7">
-        <v>3014</v>
+        <v>2861</v>
       </c>
       <c r="N15" s="7">
-        <v>35935</v>
+        <v>32538</v>
       </c>
     </row>
     <row r="16" ht="14" customHeight="1">
       <c r="A16" s="6">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="B16" s="7">
-        <v>2837</v>
+        <v>2354</v>
       </c>
       <c r="C16" s="7">
-        <v>2351</v>
+        <v>2426</v>
       </c>
       <c r="D16" s="7">
-        <v>2916</v>
+        <v>2694</v>
       </c>
       <c r="E16" s="7">
-        <v>3285</v>
+        <v>2713</v>
       </c>
       <c r="F16" s="7">
-        <v>3440</v>
+        <v>3005</v>
       </c>
       <c r="G16" s="7">
-        <v>3483</v>
+        <v>3025</v>
       </c>
       <c r="H16" s="7">
-        <v>3586</v>
+        <v>3025</v>
       </c>
       <c r="I16" s="7">
-        <v>3745</v>
+        <v>3134</v>
       </c>
       <c r="J16" s="7">
-        <v>3641</v>
+        <v>3154</v>
       </c>
       <c r="K16" s="7">
-        <v>3822</v>
+        <v>3287</v>
       </c>
       <c r="L16" s="7">
-        <v>3370</v>
+        <v>3041</v>
       </c>
       <c r="M16" s="7">
-        <v>3309</v>
+        <v>2890</v>
       </c>
       <c r="N16" s="7">
-        <v>39785</v>
+        <v>34748</v>
       </c>
     </row>
     <row r="17" ht="14" customHeight="1">
       <c r="A17" s="6">
+        <v>2017</v>
+      </c>
+      <c r="B17" s="7">
+        <v>2625</v>
+      </c>
+      <c r="C17" s="7">
+        <v>2312</v>
+      </c>
+      <c r="D17" s="7">
+        <v>2689</v>
+      </c>
+      <c r="E17" s="7">
+        <v>2770</v>
+      </c>
+      <c r="F17" s="7">
+        <v>2915</v>
+      </c>
+      <c r="G17" s="7">
+        <v>3032</v>
+      </c>
+      <c r="H17" s="7">
+        <v>3237</v>
+      </c>
+      <c r="I17" s="7">
+        <v>2990</v>
+      </c>
+      <c r="J17" s="7">
+        <v>3108</v>
+      </c>
+      <c r="K17" s="7">
+        <v>3107</v>
+      </c>
+      <c r="L17" s="7">
+        <v>2903</v>
+      </c>
+      <c r="M17" s="7">
+        <v>2872</v>
+      </c>
+      <c r="N17" s="7">
+        <v>34560</v>
+      </c>
+    </row>
+    <row r="18" ht="14" customHeight="1">
+      <c r="A18" s="6">
+        <v>2018</v>
+      </c>
+      <c r="B18" s="7">
+        <v>2631</v>
+      </c>
+      <c r="C18" s="7">
+        <v>2320</v>
+      </c>
+      <c r="D18" s="7">
+        <v>2615</v>
+      </c>
+      <c r="E18" s="7">
+        <v>2572</v>
+      </c>
+      <c r="F18" s="7">
+        <v>2977</v>
+      </c>
+      <c r="G18" s="7">
+        <v>3026</v>
+      </c>
+      <c r="H18" s="7">
+        <v>3056</v>
+      </c>
+      <c r="I18" s="7">
+        <v>3009</v>
+      </c>
+      <c r="J18" s="7">
+        <v>3064</v>
+      </c>
+      <c r="K18" s="7">
+        <v>3108</v>
+      </c>
+      <c r="L18" s="7">
+        <v>2791</v>
+      </c>
+      <c r="M18" s="7">
+        <v>2750</v>
+      </c>
+      <c r="N18" s="7">
+        <v>33919</v>
+      </c>
+    </row>
+    <row r="19" ht="14" customHeight="1">
+      <c r="A19" s="6">
+        <v>2019</v>
+      </c>
+      <c r="B19" s="7">
+        <v>2476</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2205</v>
+      </c>
+      <c r="D19" s="7">
+        <v>2544</v>
+      </c>
+      <c r="E19" s="7">
+        <v>2611</v>
+      </c>
+      <c r="F19" s="7">
+        <v>2917</v>
+      </c>
+      <c r="G19" s="7">
+        <v>2926</v>
+      </c>
+      <c r="H19" s="7">
+        <v>3037</v>
+      </c>
+      <c r="I19" s="7">
+        <v>3091</v>
+      </c>
+      <c r="J19" s="7">
+        <v>3093</v>
+      </c>
+      <c r="K19" s="7">
+        <v>2972</v>
+      </c>
+      <c r="L19" s="7">
+        <v>2841</v>
+      </c>
+      <c r="M19" s="7">
+        <v>2774</v>
+      </c>
+      <c r="N19" s="7">
+        <v>33487</v>
+      </c>
+    </row>
+    <row r="20" ht="14" customHeight="1">
+      <c r="A20" s="6">
+        <v>2020</v>
+      </c>
+      <c r="B20" s="7">
+        <v>2486</v>
+      </c>
+      <c r="C20" s="7">
+        <v>2453</v>
+      </c>
+      <c r="D20" s="7">
+        <v>2375</v>
+      </c>
+      <c r="E20" s="7">
+        <v>2130</v>
+      </c>
+      <c r="F20" s="7">
+        <v>2876</v>
+      </c>
+      <c r="G20" s="7">
+        <v>3380</v>
+      </c>
+      <c r="H20" s="7">
+        <v>3489</v>
+      </c>
+      <c r="I20" s="7">
+        <v>3539</v>
+      </c>
+      <c r="J20" s="7">
+        <v>3447</v>
+      </c>
+      <c r="K20" s="7">
+        <v>3542</v>
+      </c>
+      <c r="L20" s="7">
+        <v>3204</v>
+      </c>
+      <c r="M20" s="7">
+        <v>3014</v>
+      </c>
+      <c r="N20" s="7">
+        <v>35935</v>
+      </c>
+    </row>
+    <row r="21" ht="14" customHeight="1">
+      <c r="A21" s="6">
+        <v>2021</v>
+      </c>
+      <c r="B21" s="7">
+        <v>2837</v>
+      </c>
+      <c r="C21" s="7">
+        <v>2351</v>
+      </c>
+      <c r="D21" s="7">
+        <v>2916</v>
+      </c>
+      <c r="E21" s="7">
+        <v>3285</v>
+      </c>
+      <c r="F21" s="7">
+        <v>3440</v>
+      </c>
+      <c r="G21" s="7">
+        <v>3483</v>
+      </c>
+      <c r="H21" s="7">
+        <v>3586</v>
+      </c>
+      <c r="I21" s="7">
+        <v>3745</v>
+      </c>
+      <c r="J21" s="7">
+        <v>3641</v>
+      </c>
+      <c r="K21" s="7">
+        <v>3822</v>
+      </c>
+      <c r="L21" s="7">
+        <v>3370</v>
+      </c>
+      <c r="M21" s="7">
+        <v>3309</v>
+      </c>
+      <c r="N21" s="7">
+        <v>39785</v>
+      </c>
+    </row>
+    <row r="22" ht="14" customHeight="1">
+      <c r="A22" s="6">
         <v>2022</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B22" s="7">
         <v>2946</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C22" s="7">
         <v>2748</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D22" s="7">
         <v>3050</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E22" s="7">
         <v>2951</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F22" s="7">
         <v>3376</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G22" s="7">
         <v>3359</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H22" s="7">
         <v>3558</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I22" s="7">
         <v>3554</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J22" s="7">
         <v>3587</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K22" s="7">
         <v>3674</v>
       </c>
-      <c r="L17" s="7">
+      <c r="L22" s="7">
         <v>3200</v>
       </c>
-      <c r="M17" s="7">
+      <c r="M22" s="7">
         <v>3218</v>
       </c>
-      <c r="N17" s="7">
+      <c r="N22" s="7">
         <v>39221</v>
       </c>
     </row>
-    <row r="18" ht="14" customHeight="1">
-      <c r="A18" s="6" t="s">
+    <row r="23" ht="14" customHeight="1">
+      <c r="A23" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="7">
-        <v>25124</v>
-      </c>
-      <c r="C18" s="7">
-        <v>22643</v>
-      </c>
-      <c r="D18" s="7">
-        <v>25885</v>
-      </c>
-      <c r="E18" s="7">
-        <v>26079</v>
-      </c>
-      <c r="F18" s="7">
-        <v>29503</v>
-      </c>
-      <c r="G18" s="7">
-        <v>30296</v>
-      </c>
-      <c r="H18" s="7">
-        <v>31365</v>
-      </c>
-      <c r="I18" s="7">
-        <v>31810</v>
-      </c>
-      <c r="J18" s="7">
-        <v>31357</v>
-      </c>
-      <c r="K18" s="7">
-        <v>32181</v>
-      </c>
-      <c r="L18" s="7">
-        <v>29459</v>
-      </c>
-      <c r="M18" s="7">
-        <v>28749</v>
-      </c>
-      <c r="N18" s="7">
-        <v>344451</v>
-      </c>
-    </row>
-    <row r="19" ht="12" customHeight="1"/>
+      <c r="B23" s="7">
+        <v>36548</v>
+      </c>
+      <c r="C23" s="7">
+        <v>33233</v>
+      </c>
+      <c r="D23" s="7">
+        <v>37703</v>
+      </c>
+      <c r="E23" s="7">
+        <v>38717</v>
+      </c>
+      <c r="F23" s="7">
+        <v>43124</v>
+      </c>
+      <c r="G23" s="7">
+        <v>44057</v>
+      </c>
+      <c r="H23" s="7">
+        <v>45765</v>
+      </c>
+      <c r="I23" s="7">
+        <v>46317</v>
+      </c>
+      <c r="J23" s="7">
+        <v>45034</v>
+      </c>
+      <c r="K23" s="7">
+        <v>46207</v>
+      </c>
+      <c r="L23" s="7">
+        <v>42483</v>
+      </c>
+      <c r="M23" s="7">
+        <v>41466</v>
+      </c>
+      <c r="N23" s="7">
+        <v>500654</v>
+      </c>
+    </row>
+    <row r="24" ht="12" customHeight="1"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A6:A7"/>
@@ -955,8 +1175,8 @@
   <headerFooter>
     <oddHeader/>
     <oddFooter>Data Sources:-1 Fatality Analysis Reporting System (FARS): 2013-2021 Final File and 2022 Annual Report File (ARF) -Report Generated: Wednesday, April 17, 2024 (2:56:43 PM)+1 Fatality Analysis Reporting System (FARS): 2008-2021 Final File and 2022 Annual Report File (ARF) +Report Generated: Thursday, April 18, 2024 (10:51:35 AM) VERSION 7.2, RELEASED APR 01, 2024</oddFooter>
   </headerFooter>
 </worksheet>

</xml_diff>